<commit_message>
add dark theme cho phần của Sang
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cybersoft\Bootstrap_corpvision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71997513-65EE-4BFA-880A-CF5A9157DD23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1803F1-9E06-45B9-8376-4D3DA2553AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,29 +421,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -870,7 +848,7 @@
   <dimension ref="A1:J987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -1435,8 +1413,12 @@
       <c r="A21" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="11">
+        <v>44928</v>
+      </c>
+      <c r="C21" s="11">
+        <v>44928</v>
+      </c>
       <c r="D21" s="9">
         <v>1</v>
       </c>
@@ -2484,27 +2466,27 @@
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="D2 D4:D13">
-    <cfRule type="cellIs" dxfId="20" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="29" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="19" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="30" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="17" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="26" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="15" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="25" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
responsive aboutus, feature, services, gallery
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cybersoft\Bootstrap_corpvision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1803F1-9E06-45B9-8376-4D3DA2553AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFFE23D-0ECC-4D3E-8D82-7DB45BB4058A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="42">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -421,7 +421,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -848,7 +881,7 @@
   <dimension ref="A1:J987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -907,7 +940,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="9">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>28</v>
@@ -924,9 +957,7 @@
       <c r="I2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>39</v>
-      </c>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -1140,7 +1171,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="9">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>28</v>
@@ -1157,9 +1188,7 @@
       <c r="I10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="13" t="s">
-        <v>39</v>
-      </c>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
@@ -1172,7 +1201,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="9">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>28</v>
@@ -1189,9 +1218,7 @@
       <c r="I11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>39</v>
-      </c>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
@@ -1204,7 +1231,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="9">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>28</v>
@@ -1221,9 +1248,7 @@
       <c r="I12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="13" t="s">
-        <v>39</v>
-      </c>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
@@ -1236,7 +1261,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="9">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>28</v>
@@ -1253,9 +1278,7 @@
       <c r="I13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>39</v>
-      </c>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
@@ -2465,97 +2488,112 @@
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="D2 D4:D13">
+  <conditionalFormatting sqref="D4:D8">
+    <cfRule type="cellIs" dxfId="21" priority="32" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" dxfId="20" priority="33" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="cellIs" dxfId="19" priority="31" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" dxfId="18" priority="29" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="17" priority="30" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
-    <cfRule type="cellIs" dxfId="15" priority="26" operator="greaterThan">
+  <conditionalFormatting sqref="H21">
+    <cfRule type="cellIs" dxfId="17" priority="28" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="14" priority="25" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="27" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H24">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H24">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:H26">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:D26">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:H26">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D17 D19">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D26">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
+  <conditionalFormatting sqref="H14:H17 H19">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:H26">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="D22">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D17 D19">
+  <conditionalFormatting sqref="D18">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H17 H19">
+  <conditionalFormatting sqref="H18">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
+  <conditionalFormatting sqref="D21">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
+  <conditionalFormatting sqref="D20">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="D10:D13">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
+  <conditionalFormatting sqref="D2">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
+  <conditionalFormatting sqref="D9">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>